<commit_message>
udh selesai video materinya
</commit_message>
<xml_diff>
--- a/materiVideo/dataPenjualanMinimarket.xlsx
+++ b/materiVideo/dataPenjualanMinimarket.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,28 +480,51 @@
           <t>20251004125455018565</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>8885193814391</t>
-        </is>
+      <c r="B2" t="n">
+        <v>8885193814391</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Cemilan</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>7048</t>
-        </is>
+      <c r="D2" t="n">
+        <v>7048</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45934.53813678971</v>
+        <v>45934.53813679398</v>
       </c>
       <c r="F2" t="n">
         <v>139</v>
       </c>
       <c r="G2" t="n">
+        <v>979672</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>20251004183618700050</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8885193814391</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cemilan</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>7048</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45934.77521643614</v>
+      </c>
+      <c r="F3" t="n">
+        <v>139</v>
+      </c>
+      <c r="G3" t="n">
         <v>979672</v>
       </c>
     </row>

</xml_diff>